<commit_message>
identifier selection added and controler done.
</commit_message>
<xml_diff>
--- a/final.xlsx
+++ b/final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,7 +453,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>char</t>
+          <t>int</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -463,31 +463,31 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>&lt;CHAR_TK&gt;</t>
+          <t>&lt;INT_TK&gt;</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>(</t>
+          <t>main</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>symbol</t>
+          <t>keyword</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>&lt;PHARANTESES1_TK&gt;</t>
+          <t>&lt;MAIN_TK&gt;</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>)</t>
+          <t>(</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -497,14 +497,14 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>&lt;PHARANTESES2_TK&gt;</t>
+          <t>&lt;PHARANTESES1_TK&gt;</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>{</t>
+          <t>)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -514,99 +514,99 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>&lt;BRACKET1_TK&gt;</t>
+          <t>&lt;PHARANTESES2_TK&gt;</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>{</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>keyword</t>
+          <t>symbol</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>&lt;STRING_TK&gt;</t>
+          <t>&lt;BRACKET1_TK&gt;</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>;</t>
+          <t>int</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>symbol</t>
+          <t>keyword</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>&lt;SEMICOLON_TK&gt;</t>
+          <t>&lt;INT_TK&gt;</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>printf</t>
+          <t>1stPlace</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>keyword</t>
+          <t>identifier</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>&lt;PRINTF_TK&gt;</t>
+          <t>&lt;ID_TK, 1&gt;</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>(</t>
+          <t>=</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>symbol</t>
+          <t>operators</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>&lt;PHARANTESES1_TK&gt;</t>
+          <t>&lt;ASIGN_TK&gt;</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>"again it is valid"</t>
+          <t>100</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>string_constant</t>
+          <t>integer</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>&lt;STR_TK, "again it is valid"&gt;</t>
+          <t>&lt;INT_CONST&gt;</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>)</t>
+          <t>;</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -616,14 +616,14 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>&lt;PHARANTESES2_TK&gt;</t>
+          <t>&lt;SEMICOLON_TK&gt;</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>printf</t>
+          <t>return</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -633,48 +633,48 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>&lt;PRINTF_TK&gt;</t>
+          <t>&lt;RETURN_TK&gt;</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>(</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>symbol</t>
+          <t>integer</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>&lt;PHARANTESES1_TK&gt;</t>
+          <t>&lt;INT_CONST&gt;</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>"/*i want to find bug in the workkk*/"</t>
+          <t>;</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>string_constant</t>
+          <t>symbol</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>&lt;STR_TK, "/*i want to find bug in the workkk*/"&gt;</t>
+          <t>&lt;SEMICOLON_TK&gt;</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>)</t>
+          <t>}</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -683,57 +683,6 @@
         </is>
       </c>
       <c r="C15" t="inlineStr">
-        <is>
-          <t>&lt;PHARANTESES2_TK&gt;</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>return</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>keyword</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>&lt;RETURN_TK&gt;</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>"lexical don't give error"</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>string_constant</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>&lt;STR_TK, "lexical don't give error"&gt;</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>}</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>symbol</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
         <is>
           <t>&lt;BRACKET2_TK&gt;</t>
         </is>

</xml_diff>

<commit_message>
some bugs fixed and checked all parts
</commit_message>
<xml_diff>
--- a/final.xlsx
+++ b/final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,7 +453,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>char</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -463,24 +463,24 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>&lt;INT_TK&gt;</t>
+          <t>&lt;CHAR_TK&gt;</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>main</t>
+          <t>valid</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>keyword</t>
+          <t>identifier</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>&lt;MAIN_TK&gt;</t>
+          <t>&lt;ID_TK, 1&gt;</t>
         </is>
       </c>
     </row>
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>string</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -548,14 +548,14 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>&lt;INT_TK&gt;</t>
+          <t>&lt;STRING_TK&gt;</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1stPlace</t>
+          <t>itisvalid</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -565,7 +565,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>&lt;ID_TK, 1&gt;</t>
+          <t>&lt;ID_TK, 2&gt;</t>
         </is>
       </c>
     </row>
@@ -589,7 +589,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>4</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -623,7 +623,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>return</t>
+          <t>printf</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -633,56 +633,175 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>&lt;RETURN_TK&gt;</t>
+          <t>&lt;PRINTF_TK&gt;</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>(</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>integer</t>
+          <t>symbol</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>&lt;INT_CONST&gt;</t>
+          <t>&lt;PHARANTESES1_TK&gt;</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>;</t>
+          <t>"again it is valid"</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>symbol</t>
+          <t>string_constant</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>&lt;SEMICOLON_TK&gt;</t>
+          <t>&lt;STR_TK&gt;</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>)</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>&lt;PHARANTESES2_TK&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>printf</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>keyword</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>&lt;PRINTF_TK&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>(</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>&lt;PHARANTESES1_TK&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>"/*i want to find bug in the workkk*/"</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>string_constant</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>&lt;STR_TK&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>)</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>&lt;PHARANTESES2_TK&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>return</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>keyword</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>&lt;RETURN_TK&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>"lexical don't give error"</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>string_constant</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>&lt;STR_TK&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
           <t>}</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B22" t="inlineStr">
         <is>
           <t>symbol</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C22" t="inlineStr">
         <is>
           <t>&lt;BRACKET2_TK&gt;</t>
         </is>

</xml_diff>